<commit_message>
latest data files as of 2019-01-15 (2)
latest data files as of 2019-01-15 (2) - Test Cases Fab4
</commit_message>
<xml_diff>
--- a/src/com/data/Test Cases Fab4.xlsx
+++ b/src/com/data/Test Cases Fab4.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8361" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8361" uniqueCount="346">
   <si>
     <t>TCID</t>
   </si>
@@ -729,9 +729,6 @@
     <t>user_info</t>
   </si>
   <si>
-    <t>AJOETEST2@GMAIL.COM :: Professional Engineer :: AJ2</t>
-  </si>
-  <si>
     <t>1 :: Gas Work Piping, Devices and Meters :: Piping, traps and Valves</t>
   </si>
   <si>
@@ -1048,6 +1045,15 @@
   </si>
   <si>
     <t>1 :: AJOETEST@GMAIL.COM :: Professional Engineer :: 5546 :: Post-installed Anchors</t>
+  </si>
+  <si>
+    <t>AJOETEST2@GMAIL.COM :: Professional Engineer :: AJ2 :: APPLEROME16@GMAIL.COM</t>
+  </si>
+  <si>
+    <t>AJOETEST2@GMAIL.COM :: Professional Engineer :: AJ2V :: APPLEROME16@GMAIL.COM</t>
+  </si>
+  <si>
+    <t>Y :: APPLEROME18@GMAIL.COM</t>
   </si>
 </sst>
 </file>
@@ -2639,7 +2645,7 @@
     </row>
     <row r="40" spans="1:3" s="2" customFormat="1">
       <c r="A40" s="38" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B40" s="32"/>
       <c r="C40" s="34" t="s">
@@ -2656,7 +2662,7 @@
     </row>
     <row r="42" spans="1:3" s="2" customFormat="1">
       <c r="A42" s="38" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B42" s="32"/>
       <c r="C42" s="34" t="s">
@@ -2808,7 +2814,7 @@
     </row>
     <row r="63" spans="1:3">
       <c r="A63" s="38" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C63" s="34" t="s">
         <v>3</v>
@@ -2816,7 +2822,7 @@
     </row>
     <row r="64" spans="1:3">
       <c r="A64" s="38" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C64" s="34" t="s">
         <v>3</v>
@@ -2824,7 +2830,7 @@
     </row>
     <row r="65" spans="1:3">
       <c r="A65" s="38" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C65" s="34" t="s">
         <v>3</v>
@@ -2832,7 +2838,7 @@
     </row>
     <row r="66" spans="1:3">
       <c r="A66" s="38" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C66" s="34" t="s">
         <v>3</v>
@@ -2848,7 +2854,7 @@
     </row>
     <row r="68" spans="1:3">
       <c r="A68" s="38" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C68" s="34" t="s">
         <v>3</v>
@@ -2856,7 +2862,7 @@
     </row>
     <row r="69" spans="1:3">
       <c r="A69" s="38" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C69" s="34" t="s">
         <v>3</v>
@@ -2910,7 +2916,7 @@
     </row>
     <row r="77" spans="1:3">
       <c r="A77" s="38" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C77" s="34" t="s">
         <v>3</v>
@@ -2918,7 +2924,7 @@
     </row>
     <row r="78" spans="1:3">
       <c r="A78" s="38" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C78" s="34" t="s">
         <v>3</v>
@@ -2926,7 +2932,7 @@
     </row>
     <row r="79" spans="1:3" s="2" customFormat="1">
       <c r="A79" s="38" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B79" s="32"/>
       <c r="C79" s="34" t="s">
@@ -2935,7 +2941,7 @@
     </row>
     <row r="80" spans="1:3">
       <c r="A80" s="38" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C80" s="34" t="s">
         <v>3</v>
@@ -2943,7 +2949,7 @@
     </row>
     <row r="81" spans="1:3">
       <c r="A81" s="38" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C81" s="34" t="s">
         <v>3</v>
@@ -2951,7 +2957,7 @@
     </row>
     <row r="82" spans="1:3">
       <c r="A82" s="38" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C82" s="34" t="s">
         <v>3</v>
@@ -2959,7 +2965,7 @@
     </row>
     <row r="84" spans="1:3">
       <c r="A84" s="38" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C84" s="34" t="s">
         <v>3</v>
@@ -2967,7 +2973,7 @@
     </row>
     <row r="85" spans="1:3">
       <c r="A85" s="38" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C85" s="34" t="s">
         <v>3</v>
@@ -2975,7 +2981,7 @@
     </row>
     <row r="86" spans="1:3">
       <c r="A86" s="38" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C86" s="34" t="s">
         <v>3</v>
@@ -2988,7 +2994,7 @@
     </row>
     <row r="88" spans="1:3">
       <c r="A88" s="38" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C88" s="34" t="s">
         <v>3</v>
@@ -2996,7 +3002,7 @@
     </row>
     <row r="89" spans="1:3">
       <c r="A89" s="38" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C89" s="34" t="s">
         <v>3</v>
@@ -3022,9 +3028,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CW250"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A190" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="U1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="V192" sqref="V192"/>
+    <sheetView tabSelected="1" topLeftCell="A225" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="W1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Z242" sqref="Z242"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.140625" defaultRowHeight="12.75"/>
@@ -3337,7 +3343,7 @@
     </row>
     <row r="5" spans="1:92" s="8" customFormat="1">
       <c r="A5" s="38" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B5" s="7"/>
       <c r="E5" s="28"/>
@@ -3452,7 +3458,7 @@
         <v>27</v>
       </c>
       <c r="V6" s="16" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="W6" s="16" t="s">
         <v>28</v>
@@ -3668,19 +3674,19 @@
         <v>3</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C7" s="21" t="s">
         <v>7</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>237</v>
+        <v>343</v>
       </c>
       <c r="E7" s="19" t="s">
         <v>175</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>177</v>
@@ -3714,7 +3720,7 @@
         <v>3</v>
       </c>
       <c r="R7" s="12" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="S7" s="5" t="s">
         <v>3</v>
@@ -3723,10 +3729,10 @@
         <v>185</v>
       </c>
       <c r="U7" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="V7" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="W7" s="12" t="s">
         <v>228</v>
@@ -3842,7 +3848,7 @@
     </row>
     <row r="9" spans="1:92" s="8" customFormat="1">
       <c r="A9" s="38" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B9" s="7"/>
       <c r="E9" s="28"/>
@@ -3957,7 +3963,7 @@
         <v>27</v>
       </c>
       <c r="V10" s="16" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="W10" s="16" t="s">
         <v>28</v>
@@ -4173,19 +4179,19 @@
         <v>3</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C11" s="21" t="s">
         <v>7</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>237</v>
+        <v>343</v>
       </c>
       <c r="E11" s="19" t="s">
         <v>175</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>177</v>
@@ -4219,7 +4225,7 @@
         <v>3</v>
       </c>
       <c r="R11" s="12" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="S11" s="5" t="s">
         <v>3</v>
@@ -4228,10 +4234,10 @@
         <v>185</v>
       </c>
       <c r="U11" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="V11" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="W11" s="12" t="s">
         <v>228</v>
@@ -5296,13 +5302,13 @@
         <v>3</v>
       </c>
       <c r="B26" s="22" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C26" s="21" t="s">
         <v>7</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>237</v>
+        <v>343</v>
       </c>
       <c r="E26" s="19" t="s">
         <v>80</v>
@@ -5320,7 +5326,7 @@
         <v>3</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="K26" s="5" t="s">
         <v>123</v>
@@ -5346,7 +5352,7 @@
         <v>3</v>
       </c>
       <c r="T26" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="U26" s="5" t="s">
         <v>235</v>
@@ -5796,13 +5802,13 @@
         <v>3</v>
       </c>
       <c r="B30" s="22" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C30" s="39" t="s">
         <v>156</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>237</v>
+        <v>343</v>
       </c>
       <c r="E30" s="19" t="s">
         <v>80</v>
@@ -5820,7 +5826,7 @@
         <v>3</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="K30" s="5" t="s">
         <v>123</v>
@@ -5846,7 +5852,7 @@
         <v>3</v>
       </c>
       <c r="T30" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="U30" s="5" t="s">
         <v>129</v>
@@ -6302,7 +6308,7 @@
         <v>7</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>237</v>
+        <v>343</v>
       </c>
       <c r="E34" s="19" t="s">
         <v>80</v>
@@ -6314,13 +6320,13 @@
         <v>4</v>
       </c>
       <c r="H34" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="I34" s="5" t="s">
         <v>3</v>
       </c>
       <c r="J34" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="K34" s="5" t="s">
         <v>123</v>
@@ -6346,13 +6352,13 @@
         <v>3</v>
       </c>
       <c r="T34" s="5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="U34" s="5" t="s">
         <v>129</v>
       </c>
       <c r="V34" s="5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="W34" s="12" t="s">
         <v>228</v>
@@ -6802,7 +6808,7 @@
         <v>156</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>237</v>
+        <v>343</v>
       </c>
       <c r="E38" s="19" t="s">
         <v>80</v>
@@ -6814,13 +6820,13 @@
         <v>4</v>
       </c>
       <c r="H38" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="I38" s="5" t="s">
         <v>3</v>
       </c>
       <c r="J38" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="K38" s="5" t="s">
         <v>123</v>
@@ -6846,13 +6852,13 @@
         <v>3</v>
       </c>
       <c r="T38" s="5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="U38" s="5" t="s">
         <v>129</v>
       </c>
       <c r="V38" s="5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="W38" s="12" t="s">
         <v>228</v>
@@ -7296,13 +7302,13 @@
         <v>3</v>
       </c>
       <c r="B42" s="22" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C42" s="21" t="s">
         <v>7</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>237</v>
+        <v>343</v>
       </c>
       <c r="E42" s="19" t="s">
         <v>80</v>
@@ -7320,7 +7326,7 @@
         <v>3</v>
       </c>
       <c r="J42" s="5" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="K42" s="5" t="s">
         <v>123</v>
@@ -7346,13 +7352,13 @@
         <v>3</v>
       </c>
       <c r="T42" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="U42" s="5" t="s">
         <v>126</v>
       </c>
       <c r="V42" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="W42" s="12" t="s">
         <v>229</v>
@@ -7796,13 +7802,13 @@
         <v>3</v>
       </c>
       <c r="B46" s="22" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C46" s="39" t="s">
         <v>156</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>237</v>
+        <v>343</v>
       </c>
       <c r="E46" s="19" t="s">
         <v>80</v>
@@ -7820,7 +7826,7 @@
         <v>3</v>
       </c>
       <c r="J46" s="5" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="K46" s="5" t="s">
         <v>123</v>
@@ -7846,13 +7852,13 @@
         <v>3</v>
       </c>
       <c r="T46" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="U46" s="5" t="s">
         <v>126</v>
       </c>
       <c r="V46" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="W46" s="12" t="s">
         <v>229</v>
@@ -8291,18 +8297,18 @@
         <v>99</v>
       </c>
     </row>
-    <row r="50" spans="1:92" s="5" customFormat="1" ht="38.25">
+    <row r="50" spans="1:92" s="5" customFormat="1" ht="75">
       <c r="A50" s="27" t="s">
         <v>3</v>
       </c>
       <c r="B50" s="22" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C50" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="D50" s="5" t="s">
-        <v>237</v>
+      <c r="D50" s="41" t="s">
+        <v>344</v>
       </c>
       <c r="E50" s="19" t="s">
         <v>80</v>
@@ -8314,13 +8320,13 @@
         <v>4</v>
       </c>
       <c r="H50" s="5" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="I50" s="5" t="s">
         <v>3</v>
       </c>
       <c r="J50" s="5" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="K50" s="5" t="s">
         <v>123</v>
@@ -8346,13 +8352,13 @@
         <v>3</v>
       </c>
       <c r="T50" s="5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="U50" s="5" t="s">
         <v>145</v>
       </c>
       <c r="V50" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="W50" s="12" t="s">
         <v>228</v>
@@ -8796,13 +8802,13 @@
         <v>3</v>
       </c>
       <c r="B54" s="22" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C54" s="39" t="s">
         <v>156</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>237</v>
+        <v>343</v>
       </c>
       <c r="E54" s="19" t="s">
         <v>80</v>
@@ -8814,13 +8820,13 @@
         <v>4</v>
       </c>
       <c r="H54" s="5" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="I54" s="5" t="s">
         <v>3</v>
       </c>
       <c r="J54" s="5" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="K54" s="5" t="s">
         <v>123</v>
@@ -8846,13 +8852,13 @@
         <v>3</v>
       </c>
       <c r="T54" s="5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="U54" s="5" t="s">
         <v>145</v>
       </c>
       <c r="V54" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="W54" s="12" t="s">
         <v>228</v>
@@ -9296,13 +9302,13 @@
         <v>3</v>
       </c>
       <c r="B58" s="22" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C58" s="21" t="s">
         <v>7</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>237</v>
+        <v>343</v>
       </c>
       <c r="E58" s="19" t="s">
         <v>80</v>
@@ -9314,13 +9320,13 @@
         <v>4</v>
       </c>
       <c r="H58" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="I58" s="5" t="s">
         <v>3</v>
       </c>
       <c r="J58" s="5" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="K58" s="5" t="s">
         <v>123</v>
@@ -9346,13 +9352,13 @@
         <v>3</v>
       </c>
       <c r="T58" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="U58" s="5" t="s">
         <v>126</v>
       </c>
       <c r="V58" s="5" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="W58" s="12" t="s">
         <v>228</v>
@@ -9796,13 +9802,13 @@
         <v>3</v>
       </c>
       <c r="B62" s="22" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C62" s="39" t="s">
         <v>156</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>237</v>
+        <v>343</v>
       </c>
       <c r="E62" s="19" t="s">
         <v>80</v>
@@ -9814,13 +9820,13 @@
         <v>4</v>
       </c>
       <c r="H62" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="I62" s="5" t="s">
         <v>3</v>
       </c>
       <c r="J62" s="5" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="K62" s="5" t="s">
         <v>123</v>
@@ -9846,13 +9852,13 @@
         <v>3</v>
       </c>
       <c r="T62" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="U62" s="5" t="s">
         <v>126</v>
       </c>
       <c r="V62" s="5" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="W62" s="12" t="s">
         <v>228</v>
@@ -10302,7 +10308,7 @@
         <v>7</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>237</v>
+        <v>343</v>
       </c>
       <c r="E66" s="19" t="s">
         <v>80</v>
@@ -10314,13 +10320,13 @@
         <v>4</v>
       </c>
       <c r="H66" s="5" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="I66" s="5" t="s">
         <v>3</v>
       </c>
       <c r="J66" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="K66" s="5" t="s">
         <v>123</v>
@@ -10346,13 +10352,13 @@
         <v>3</v>
       </c>
       <c r="T66" s="5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="U66" s="5" t="s">
         <v>129</v>
       </c>
       <c r="V66" s="5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="W66" s="12" t="s">
         <v>228</v>
@@ -10802,7 +10808,7 @@
         <v>156</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>237</v>
+        <v>343</v>
       </c>
       <c r="E70" s="19" t="s">
         <v>80</v>
@@ -10814,13 +10820,13 @@
         <v>4</v>
       </c>
       <c r="H70" s="5" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="I70" s="5" t="s">
         <v>3</v>
       </c>
       <c r="J70" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="K70" s="5" t="s">
         <v>123</v>
@@ -10846,13 +10852,13 @@
         <v>3</v>
       </c>
       <c r="T70" s="5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="U70" s="5" t="s">
         <v>129</v>
       </c>
       <c r="V70" s="5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="W70" s="12" t="s">
         <v>228</v>
@@ -10965,7 +10971,7 @@
     </row>
     <row r="72" spans="1:92" s="8" customFormat="1">
       <c r="A72" s="38" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B72" s="7"/>
       <c r="E72" s="7"/>
@@ -11296,13 +11302,13 @@
         <v>3</v>
       </c>
       <c r="B74" s="22" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C74" s="21" t="s">
         <v>7</v>
       </c>
       <c r="D74" s="5" t="s">
-        <v>237</v>
+        <v>343</v>
       </c>
       <c r="E74" s="19" t="s">
         <v>80</v>
@@ -11314,13 +11320,13 @@
         <v>4</v>
       </c>
       <c r="H74" s="5" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="I74" s="5" t="s">
         <v>3</v>
       </c>
       <c r="J74" s="5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="K74" s="5" t="s">
         <v>123</v>
@@ -11346,13 +11352,13 @@
         <v>3</v>
       </c>
       <c r="T74" s="5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="U74" s="5" t="s">
         <v>145</v>
       </c>
       <c r="V74" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="W74" s="12" t="s">
         <v>228</v>
@@ -11465,7 +11471,7 @@
     </row>
     <row r="76" spans="1:92" s="8" customFormat="1">
       <c r="A76" s="38" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B76" s="7"/>
       <c r="E76" s="7"/>
@@ -11796,13 +11802,13 @@
         <v>3</v>
       </c>
       <c r="B78" s="22" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C78" s="39" t="s">
         <v>156</v>
       </c>
       <c r="D78" s="5" t="s">
-        <v>237</v>
+        <v>343</v>
       </c>
       <c r="E78" s="19" t="s">
         <v>80</v>
@@ -11814,13 +11820,13 @@
         <v>4</v>
       </c>
       <c r="H78" s="5" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="I78" s="5" t="s">
         <v>3</v>
       </c>
       <c r="J78" s="5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="K78" s="5" t="s">
         <v>123</v>
@@ -11846,13 +11852,13 @@
         <v>3</v>
       </c>
       <c r="T78" s="5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="U78" s="5" t="s">
         <v>145</v>
       </c>
       <c r="V78" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="W78" s="12" t="s">
         <v>228</v>
@@ -11965,7 +11971,7 @@
     </row>
     <row r="80" spans="1:92" s="8" customFormat="1">
       <c r="A80" s="38" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B80" s="7"/>
       <c r="E80" s="7"/>
@@ -12296,13 +12302,13 @@
         <v>3</v>
       </c>
       <c r="B82" s="22" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C82" s="21" t="s">
         <v>7</v>
       </c>
       <c r="D82" s="5" t="s">
-        <v>237</v>
+        <v>343</v>
       </c>
       <c r="E82" s="19" t="s">
         <v>80</v>
@@ -12314,13 +12320,13 @@
         <v>4</v>
       </c>
       <c r="H82" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="I82" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="J82" s="5" t="s">
         <v>275</v>
-      </c>
-      <c r="I82" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="J82" s="5" t="s">
-        <v>276</v>
       </c>
       <c r="K82" s="5" t="s">
         <v>123</v>
@@ -12346,13 +12352,13 @@
         <v>3</v>
       </c>
       <c r="T82" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="U82" s="5" t="s">
         <v>126</v>
       </c>
       <c r="V82" s="5" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="W82" s="12" t="s">
         <v>229</v>
@@ -12465,7 +12471,7 @@
     </row>
     <row r="84" spans="1:92" s="8" customFormat="1">
       <c r="A84" s="38" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B84" s="7"/>
       <c r="E84" s="7"/>
@@ -12796,13 +12802,13 @@
         <v>3</v>
       </c>
       <c r="B86" s="22" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C86" s="39" t="s">
         <v>156</v>
       </c>
       <c r="D86" s="5" t="s">
-        <v>237</v>
+        <v>343</v>
       </c>
       <c r="E86" s="19" t="s">
         <v>80</v>
@@ -12814,13 +12820,13 @@
         <v>4</v>
       </c>
       <c r="H86" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="I86" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="J86" s="5" t="s">
         <v>275</v>
-      </c>
-      <c r="I86" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="J86" s="5" t="s">
-        <v>276</v>
       </c>
       <c r="K86" s="5" t="s">
         <v>123</v>
@@ -12846,13 +12852,13 @@
         <v>3</v>
       </c>
       <c r="T86" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="U86" s="5" t="s">
         <v>126</v>
       </c>
       <c r="V86" s="5" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="W86" s="12" t="s">
         <v>229</v>
@@ -12965,7 +12971,7 @@
     </row>
     <row r="88" spans="1:92" s="8" customFormat="1">
       <c r="A88" s="38" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B88" s="7"/>
       <c r="E88" s="7"/>
@@ -13296,13 +13302,13 @@
         <v>3</v>
       </c>
       <c r="B90" s="22" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C90" s="21" t="s">
         <v>7</v>
       </c>
       <c r="D90" s="5" t="s">
-        <v>237</v>
+        <v>343</v>
       </c>
       <c r="E90" s="19" t="s">
         <v>80</v>
@@ -13314,13 +13320,13 @@
         <v>4</v>
       </c>
       <c r="H90" s="5" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="I90" s="5" t="s">
         <v>3</v>
       </c>
       <c r="J90" s="5" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="K90" s="5" t="s">
         <v>123</v>
@@ -13346,13 +13352,13 @@
         <v>3</v>
       </c>
       <c r="T90" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="U90" s="5" t="s">
         <v>126</v>
       </c>
       <c r="V90" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="W90" s="12" t="s">
         <v>228</v>
@@ -13465,7 +13471,7 @@
     </row>
     <row r="92" spans="1:92" s="8" customFormat="1">
       <c r="A92" s="38" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B92" s="7"/>
       <c r="E92" s="7"/>
@@ -13796,13 +13802,13 @@
         <v>3</v>
       </c>
       <c r="B94" s="22" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C94" s="39" t="s">
         <v>156</v>
       </c>
       <c r="D94" s="5" t="s">
-        <v>237</v>
+        <v>343</v>
       </c>
       <c r="E94" s="19" t="s">
         <v>80</v>
@@ -13814,13 +13820,13 @@
         <v>4</v>
       </c>
       <c r="H94" s="5" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="I94" s="5" t="s">
         <v>3</v>
       </c>
       <c r="J94" s="5" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="K94" s="5" t="s">
         <v>123</v>
@@ -13846,13 +13852,13 @@
         <v>3</v>
       </c>
       <c r="T94" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="U94" s="5" t="s">
         <v>126</v>
       </c>
       <c r="V94" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="W94" s="12" t="s">
         <v>228</v>
@@ -14302,7 +14308,7 @@
         <v>7</v>
       </c>
       <c r="D98" s="5" t="s">
-        <v>237</v>
+        <v>343</v>
       </c>
       <c r="E98" s="19" t="s">
         <v>152</v>
@@ -14314,13 +14320,13 @@
         <v>4</v>
       </c>
       <c r="H98" s="5" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="I98" s="5" t="s">
         <v>3</v>
       </c>
       <c r="J98" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="K98" s="5" t="s">
         <v>123</v>
@@ -14352,7 +14358,7 @@
         <v>153</v>
       </c>
       <c r="V98" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="W98" s="12" t="s">
         <v>228</v>
@@ -14802,7 +14808,7 @@
         <v>156</v>
       </c>
       <c r="D102" s="5" t="s">
-        <v>237</v>
+        <v>343</v>
       </c>
       <c r="E102" s="19" t="s">
         <v>152</v>
@@ -14814,13 +14820,13 @@
         <v>4</v>
       </c>
       <c r="H102" s="5" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="I102" s="5" t="s">
         <v>3</v>
       </c>
       <c r="J102" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="K102" s="5" t="s">
         <v>123</v>
@@ -14852,7 +14858,7 @@
         <v>153</v>
       </c>
       <c r="V102" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="W102" s="12" t="s">
         <v>228</v>
@@ -15296,13 +15302,13 @@
         <v>3</v>
       </c>
       <c r="B106" s="22" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C106" s="21" t="s">
         <v>7</v>
       </c>
       <c r="D106" s="5" t="s">
-        <v>237</v>
+        <v>343</v>
       </c>
       <c r="E106" s="19" t="s">
         <v>81</v>
@@ -15314,13 +15320,13 @@
         <v>4</v>
       </c>
       <c r="H106" s="5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="I106" s="5" t="s">
         <v>3</v>
       </c>
       <c r="J106" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="K106" s="5" t="s">
         <v>123</v>
@@ -15346,13 +15352,13 @@
         <v>3</v>
       </c>
       <c r="T106" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="U106" s="5" t="s">
         <v>137</v>
       </c>
       <c r="V106" s="5" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="W106" s="12" t="s">
         <v>229</v>
@@ -15790,13 +15796,13 @@
         <v>3</v>
       </c>
       <c r="B110" s="22" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C110" s="39" t="s">
         <v>156</v>
       </c>
       <c r="D110" s="5" t="s">
-        <v>237</v>
+        <v>343</v>
       </c>
       <c r="E110" s="19" t="s">
         <v>81</v>
@@ -15808,13 +15814,13 @@
         <v>4</v>
       </c>
       <c r="H110" s="5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="I110" s="5" t="s">
         <v>3</v>
       </c>
       <c r="J110" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="K110" s="5" t="s">
         <v>123</v>
@@ -15840,13 +15846,13 @@
         <v>3</v>
       </c>
       <c r="T110" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="U110" s="5" t="s">
         <v>137</v>
       </c>
       <c r="V110" s="5" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="W110" s="12" t="s">
         <v>229</v>
@@ -16290,7 +16296,7 @@
         <v>7</v>
       </c>
       <c r="D114" s="5" t="s">
-        <v>237</v>
+        <v>343</v>
       </c>
       <c r="E114" s="19" t="s">
         <v>81</v>
@@ -16302,13 +16308,13 @@
         <v>4</v>
       </c>
       <c r="H114" s="5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="I114" s="5" t="s">
         <v>3</v>
       </c>
       <c r="J114" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="K114" s="5" t="s">
         <v>123</v>
@@ -16340,7 +16346,7 @@
         <v>137</v>
       </c>
       <c r="V114" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="W114" s="12" t="s">
         <v>228</v>
@@ -16787,7 +16793,7 @@
         <v>7</v>
       </c>
       <c r="D118" s="5" t="s">
-        <v>237</v>
+        <v>343</v>
       </c>
       <c r="E118" s="19" t="s">
         <v>81</v>
@@ -16799,13 +16805,13 @@
         <v>4</v>
       </c>
       <c r="H118" s="5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="I118" s="5" t="s">
         <v>3</v>
       </c>
       <c r="J118" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="K118" s="5" t="s">
         <v>123</v>
@@ -16837,7 +16843,7 @@
         <v>137</v>
       </c>
       <c r="V118" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="W118" s="12" t="s">
         <v>228</v>
@@ -17284,7 +17290,7 @@
         <v>156</v>
       </c>
       <c r="D122" s="5" t="s">
-        <v>237</v>
+        <v>343</v>
       </c>
       <c r="E122" s="19" t="s">
         <v>81</v>
@@ -17296,13 +17302,13 @@
         <v>4</v>
       </c>
       <c r="H122" s="5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="I122" s="5" t="s">
         <v>3</v>
       </c>
       <c r="J122" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="K122" s="5" t="s">
         <v>123</v>
@@ -17334,7 +17340,7 @@
         <v>137</v>
       </c>
       <c r="V122" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="W122" s="12" t="s">
         <v>228</v>
@@ -17778,7 +17784,7 @@
         <v>7</v>
       </c>
       <c r="D126" s="5" t="s">
-        <v>237</v>
+        <v>343</v>
       </c>
       <c r="E126" s="19" t="s">
         <v>81</v>
@@ -17790,13 +17796,13 @@
         <v>4</v>
       </c>
       <c r="H126" s="5" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="I126" s="5" t="s">
         <v>3</v>
       </c>
       <c r="J126" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="K126" s="5" t="s">
         <v>123</v>
@@ -17828,7 +17834,7 @@
         <v>137</v>
       </c>
       <c r="V126" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="W126" s="12" t="s">
         <v>228</v>
@@ -18272,7 +18278,7 @@
         <v>156</v>
       </c>
       <c r="D130" s="5" t="s">
-        <v>237</v>
+        <v>343</v>
       </c>
       <c r="E130" s="19" t="s">
         <v>81</v>
@@ -18284,13 +18290,13 @@
         <v>4</v>
       </c>
       <c r="H130" s="5" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="I130" s="5" t="s">
         <v>3</v>
       </c>
       <c r="J130" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="K130" s="5" t="s">
         <v>123</v>
@@ -18322,7 +18328,7 @@
         <v>137</v>
       </c>
       <c r="V130" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="W130" s="12" t="s">
         <v>228</v>
@@ -18902,13 +18908,13 @@
         <v>7</v>
       </c>
       <c r="D136" s="5" t="s">
-        <v>237</v>
+        <v>343</v>
       </c>
       <c r="E136" s="19" t="s">
         <v>208</v>
       </c>
       <c r="F136" s="5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="G136" s="5" t="s">
         <v>177</v>
@@ -18949,7 +18955,7 @@
         <v>209</v>
       </c>
       <c r="U136" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="V136" s="5" t="s">
         <v>181</v>
@@ -19068,7 +19074,7 @@
     </row>
     <row r="138" spans="1:92" s="8" customFormat="1">
       <c r="A138" s="38" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B138" s="7"/>
       <c r="E138" s="28"/>
@@ -19399,19 +19405,19 @@
         <v>3</v>
       </c>
       <c r="B140" s="22" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C140" s="39" t="s">
         <v>156</v>
       </c>
       <c r="D140" s="5" t="s">
-        <v>237</v>
+        <v>343</v>
       </c>
       <c r="E140" s="19" t="s">
         <v>208</v>
       </c>
       <c r="F140" s="5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G140" s="5" t="s">
         <v>177</v>
@@ -19452,7 +19458,7 @@
         <v>209</v>
       </c>
       <c r="U140" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="V140" s="5" t="s">
         <v>181</v>
@@ -19897,7 +19903,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="144" spans="1:92" s="5" customFormat="1" ht="38.25">
+    <row r="144" spans="1:92" s="5" customFormat="1" ht="63.75">
       <c r="A144" s="27" t="s">
         <v>3</v>
       </c>
@@ -19905,16 +19911,16 @@
         <v>207</v>
       </c>
       <c r="C144" s="21" t="s">
+        <v>322</v>
+      </c>
+      <c r="D144" s="5" t="s">
+        <v>343</v>
+      </c>
+      <c r="E144" s="19" t="s">
+        <v>321</v>
+      </c>
+      <c r="F144" s="5" t="s">
         <v>323</v>
-      </c>
-      <c r="D144" s="5" t="s">
-        <v>237</v>
-      </c>
-      <c r="E144" s="19" t="s">
-        <v>322</v>
-      </c>
-      <c r="F144" s="5" t="s">
-        <v>324</v>
       </c>
       <c r="G144" s="5" t="s">
         <v>177</v>
@@ -19936,7 +19942,7 @@
         <v>180</v>
       </c>
       <c r="N144" s="12" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="O144" s="12" t="s">
         <v>197</v>
@@ -19955,7 +19961,7 @@
         <v>209</v>
       </c>
       <c r="U144" s="5" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="V144" s="5" t="s">
         <v>181</v>
@@ -19966,7 +19972,7 @@
       <c r="X144" s="12"/>
       <c r="Y144" s="12"/>
       <c r="Z144" s="12" t="s">
-        <v>3</v>
+        <v>345</v>
       </c>
       <c r="AA144" s="12" t="s">
         <v>29</v>
@@ -20074,7 +20080,7 @@
     </row>
     <row r="146" spans="1:92" s="8" customFormat="1">
       <c r="A146" s="38" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B146" s="7"/>
       <c r="E146" s="28"/>
@@ -20405,19 +20411,19 @@
         <v>3</v>
       </c>
       <c r="B148" s="22" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C148" s="39" t="s">
         <v>156</v>
       </c>
       <c r="D148" s="5" t="s">
-        <v>237</v>
+        <v>343</v>
       </c>
       <c r="E148" s="19" t="s">
         <v>208</v>
       </c>
       <c r="F148" s="5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G148" s="5" t="s">
         <v>177</v>
@@ -20458,7 +20464,7 @@
         <v>209</v>
       </c>
       <c r="U148" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="V148" s="5" t="s">
         <v>181</v>
@@ -20914,13 +20920,13 @@
         <v>7</v>
       </c>
       <c r="D152" s="5" t="s">
-        <v>237</v>
+        <v>343</v>
       </c>
       <c r="E152" s="19" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F152" s="5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="G152" s="5" t="s">
         <v>177</v>
@@ -20961,7 +20967,7 @@
         <v>191</v>
       </c>
       <c r="U152" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="V152" s="5" t="s">
         <v>181</v>
@@ -21417,13 +21423,13 @@
         <v>156</v>
       </c>
       <c r="D156" s="5" t="s">
-        <v>237</v>
+        <v>343</v>
       </c>
       <c r="E156" s="19" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F156" s="5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G156" s="5" t="s">
         <v>177</v>
@@ -21464,7 +21470,7 @@
         <v>191</v>
       </c>
       <c r="U156" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="V156" s="5" t="s">
         <v>181</v>
@@ -21920,13 +21926,13 @@
         <v>7</v>
       </c>
       <c r="D160" s="5" t="s">
-        <v>237</v>
+        <v>343</v>
       </c>
       <c r="E160" s="19" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F160" s="5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="G160" s="5" t="s">
         <v>177</v>
@@ -21967,7 +21973,7 @@
         <v>198</v>
       </c>
       <c r="U160" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="V160" s="5" t="s">
         <v>181</v>
@@ -22423,13 +22429,13 @@
         <v>156</v>
       </c>
       <c r="D164" s="5" t="s">
-        <v>237</v>
+        <v>343</v>
       </c>
       <c r="E164" s="19" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F164" s="5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G164" s="5" t="s">
         <v>177</v>
@@ -22470,7 +22476,7 @@
         <v>198</v>
       </c>
       <c r="U164" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="V164" s="5" t="s">
         <v>181</v>
@@ -22926,13 +22932,13 @@
         <v>7</v>
       </c>
       <c r="D168" s="5" t="s">
-        <v>237</v>
+        <v>343</v>
       </c>
       <c r="E168" s="19" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F168" s="5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="G168" s="5" t="s">
         <v>177</v>
@@ -22973,7 +22979,7 @@
         <v>198</v>
       </c>
       <c r="U168" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="V168" s="5" t="s">
         <v>181</v>
@@ -23429,13 +23435,13 @@
         <v>156</v>
       </c>
       <c r="D172" s="5" t="s">
-        <v>237</v>
+        <v>343</v>
       </c>
       <c r="E172" s="19" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F172" s="5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G172" s="5" t="s">
         <v>177</v>
@@ -23476,7 +23482,7 @@
         <v>198</v>
       </c>
       <c r="U172" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="V172" s="5" t="s">
         <v>181</v>
@@ -23921,7 +23927,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="176" spans="1:92" s="5" customFormat="1" ht="38.25">
+    <row r="176" spans="1:92" s="5" customFormat="1" ht="63.75">
       <c r="A176" s="27" t="s">
         <v>3</v>
       </c>
@@ -23929,16 +23935,16 @@
         <v>190</v>
       </c>
       <c r="C176" s="21" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D176" s="5" t="s">
-        <v>237</v>
+        <v>343</v>
       </c>
       <c r="E176" s="19" t="s">
+        <v>326</v>
+      </c>
+      <c r="F176" s="5" t="s">
         <v>327</v>
-      </c>
-      <c r="F176" s="5" t="s">
-        <v>328</v>
       </c>
       <c r="G176" s="5" t="s">
         <v>177</v>
@@ -23960,7 +23966,7 @@
         <v>180</v>
       </c>
       <c r="N176" s="12" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="O176" s="12"/>
       <c r="P176" s="12" t="s">
@@ -23979,7 +23985,7 @@
         <v>191</v>
       </c>
       <c r="U176" s="5" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="V176" s="5" t="s">
         <v>181</v>
@@ -23990,7 +23996,7 @@
       <c r="X176" s="12"/>
       <c r="Y176" s="12"/>
       <c r="Z176" s="12" t="s">
-        <v>3</v>
+        <v>345</v>
       </c>
       <c r="AA176" s="12" t="s">
         <v>29</v>
@@ -24435,13 +24441,13 @@
         <v>156</v>
       </c>
       <c r="D180" s="5" t="s">
-        <v>237</v>
+        <v>343</v>
       </c>
       <c r="E180" s="19" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F180" s="5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G180" s="5" t="s">
         <v>177</v>
@@ -24482,7 +24488,7 @@
         <v>191</v>
       </c>
       <c r="U180" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="V180" s="5" t="s">
         <v>181</v>
@@ -24601,7 +24607,7 @@
     </row>
     <row r="182" spans="1:92" s="8" customFormat="1">
       <c r="A182" s="38" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B182" s="7"/>
       <c r="E182" s="28"/>
@@ -24932,19 +24938,19 @@
         <v>3</v>
       </c>
       <c r="B184" s="22" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C184" s="21" t="s">
         <v>7</v>
       </c>
       <c r="D184" s="5" t="s">
-        <v>237</v>
+        <v>343</v>
       </c>
       <c r="E184" s="19" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F184" s="5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="G184" s="5" t="s">
         <v>177</v>
@@ -24985,7 +24991,7 @@
         <v>198</v>
       </c>
       <c r="U184" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="V184" s="5" t="s">
         <v>181</v>
@@ -25104,7 +25110,7 @@
     </row>
     <row r="186" spans="1:92" s="8" customFormat="1">
       <c r="A186" s="38" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B186" s="7"/>
       <c r="E186" s="28"/>
@@ -25435,19 +25441,19 @@
         <v>3</v>
       </c>
       <c r="B188" s="22" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C188" s="39" t="s">
         <v>156</v>
       </c>
       <c r="D188" s="5" t="s">
-        <v>237</v>
+        <v>343</v>
       </c>
       <c r="E188" s="19" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F188" s="5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G188" s="5" t="s">
         <v>177</v>
@@ -25472,7 +25478,7 @@
         <v>3</v>
       </c>
       <c r="O188" s="12" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="P188" s="12" t="s">
         <v>122</v>
@@ -25488,7 +25494,7 @@
         <v>198</v>
       </c>
       <c r="U188" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="V188" s="5" t="s">
         <v>181</v>
@@ -25607,7 +25613,7 @@
     </row>
     <row r="190" spans="1:92" s="8" customFormat="1">
       <c r="A190" s="38" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B190" s="7"/>
       <c r="E190" s="28"/>
@@ -25938,31 +25944,31 @@
         <v>3</v>
       </c>
       <c r="B192" s="22" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C192" s="21" t="s">
         <v>7</v>
       </c>
       <c r="D192" s="41" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E192" s="40" t="s">
+        <v>335</v>
+      </c>
+      <c r="F192" s="5" t="s">
         <v>336</v>
-      </c>
-      <c r="F192" s="5" t="s">
-        <v>337</v>
       </c>
       <c r="G192" s="5" t="s">
         <v>177</v>
       </c>
       <c r="H192" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="I192" s="5" t="s">
         <v>3</v>
       </c>
       <c r="J192" s="5" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="K192" s="5" t="s">
         <v>178</v>
@@ -25972,10 +25978,10 @@
         <v>180</v>
       </c>
       <c r="N192" s="12" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="O192" s="12" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="P192" s="12" t="s">
         <v>122</v>
@@ -25989,10 +25995,10 @@
         <v>198</v>
       </c>
       <c r="U192" s="5" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="V192" s="5" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="W192" s="12" t="s">
         <v>228</v>
@@ -26000,13 +26006,13 @@
       <c r="X192" s="12"/>
       <c r="Y192" s="12"/>
       <c r="Z192" s="12" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="AA192" s="42" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="AB192" s="42" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="AC192" s="12" t="s">
         <v>3</v>
@@ -26108,7 +26114,7 @@
     </row>
     <row r="194" spans="1:92" s="8" customFormat="1">
       <c r="A194" s="38" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B194" s="7"/>
       <c r="E194" s="28"/>
@@ -26439,25 +26445,25 @@
         <v>3</v>
       </c>
       <c r="B196" s="22" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C196" s="39" t="s">
         <v>156</v>
       </c>
       <c r="D196" s="5" t="s">
-        <v>237</v>
+        <v>343</v>
       </c>
       <c r="E196" s="19" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F196" s="5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G196" s="5" t="s">
         <v>177</v>
       </c>
       <c r="H196" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="I196" s="5" t="s">
         <v>3</v>
@@ -26492,7 +26498,7 @@
         <v>198</v>
       </c>
       <c r="U196" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="V196" s="5" t="s">
         <v>181</v>
@@ -26948,13 +26954,13 @@
         <v>7</v>
       </c>
       <c r="D200" s="5" t="s">
-        <v>237</v>
+        <v>343</v>
       </c>
       <c r="E200" s="19" t="s">
         <v>175</v>
       </c>
       <c r="F200" s="5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="G200" s="5" t="s">
         <v>177</v>
@@ -26988,7 +26994,7 @@
         <v>3</v>
       </c>
       <c r="R200" s="12" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="S200" s="5" t="s">
         <v>3</v>
@@ -26997,10 +27003,10 @@
         <v>185</v>
       </c>
       <c r="U200" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="V200" s="5" t="s">
         <v>250</v>
-      </c>
-      <c r="V200" s="5" t="s">
-        <v>251</v>
       </c>
       <c r="W200" s="12" t="s">
         <v>228</v>
@@ -27447,19 +27453,19 @@
         <v>3</v>
       </c>
       <c r="B204" s="22" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C204" s="39" t="s">
         <v>156</v>
       </c>
       <c r="D204" s="5" t="s">
-        <v>237</v>
+        <v>343</v>
       </c>
       <c r="E204" s="19" t="s">
         <v>175</v>
       </c>
       <c r="F204" s="5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G204" s="5" t="s">
         <v>177</v>
@@ -27493,7 +27499,7 @@
         <v>3</v>
       </c>
       <c r="R204" s="12" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="S204" s="5" t="s">
         <v>3</v>
@@ -27502,10 +27508,10 @@
         <v>185</v>
       </c>
       <c r="U204" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="V204" s="5" t="s">
         <v>250</v>
-      </c>
-      <c r="V204" s="5" t="s">
-        <v>251</v>
       </c>
       <c r="W204" s="12" t="s">
         <v>228</v>
@@ -27947,7 +27953,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="208" spans="1:92" s="5" customFormat="1" ht="38.25">
+    <row r="208" spans="1:92" s="5" customFormat="1" ht="63.75">
       <c r="A208" s="27" t="s">
         <v>3</v>
       </c>
@@ -27955,16 +27961,16 @@
         <v>176</v>
       </c>
       <c r="C208" s="21" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D208" s="5" t="s">
-        <v>237</v>
+        <v>343</v>
       </c>
       <c r="E208" s="19" t="s">
         <v>175</v>
       </c>
       <c r="F208" s="5" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G208" s="5" t="s">
         <v>177</v>
@@ -27998,7 +28004,7 @@
         <v>3</v>
       </c>
       <c r="R208" s="12" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="S208" s="5" t="s">
         <v>3</v>
@@ -28007,10 +28013,10 @@
         <v>185</v>
       </c>
       <c r="U208" s="5" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="V208" s="5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="W208" s="12" t="s">
         <v>228</v>
@@ -28018,7 +28024,7 @@
       <c r="X208" s="12"/>
       <c r="Y208" s="12"/>
       <c r="Z208" s="12" t="s">
-        <v>3</v>
+        <v>345</v>
       </c>
       <c r="AA208" s="12" t="s">
         <v>29</v>
@@ -28463,13 +28469,13 @@
         <v>156</v>
       </c>
       <c r="D212" s="5" t="s">
-        <v>237</v>
+        <v>343</v>
       </c>
       <c r="E212" s="19" t="s">
         <v>175</v>
       </c>
       <c r="F212" s="5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G212" s="5" t="s">
         <v>177</v>
@@ -28503,7 +28509,7 @@
         <v>3</v>
       </c>
       <c r="R212" s="12" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="S212" s="5" t="s">
         <v>3</v>
@@ -28512,10 +28518,10 @@
         <v>185</v>
       </c>
       <c r="U212" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="V212" s="5" t="s">
         <v>250</v>
-      </c>
-      <c r="V212" s="5" t="s">
-        <v>251</v>
       </c>
       <c r="W212" s="12" t="s">
         <v>228</v>
@@ -28631,7 +28637,7 @@
     </row>
     <row r="214" spans="1:92" s="8" customFormat="1">
       <c r="A214" s="38" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B214" s="7"/>
       <c r="E214" s="28"/>
@@ -28692,13 +28698,13 @@
         <v>17</v>
       </c>
       <c r="D215" s="13" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E215" s="6" t="s">
         <v>79</v>
       </c>
       <c r="F215" s="13" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="G215" s="13" t="s">
         <v>115</v>
@@ -28962,19 +28968,19 @@
         <v>3</v>
       </c>
       <c r="B216" s="22" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C216" s="21" t="s">
         <v>7</v>
       </c>
       <c r="D216" s="20" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E216" s="19" t="s">
         <v>3</v>
       </c>
       <c r="F216" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="G216" s="5" t="s">
         <v>177</v>
@@ -29008,7 +29014,7 @@
         <v>3</v>
       </c>
       <c r="R216" s="12" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="S216" s="5" t="s">
         <v>3</v>
@@ -29017,10 +29023,10 @@
         <v>185</v>
       </c>
       <c r="U216" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="V216" s="5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="W216" s="12" t="s">
         <v>228</v>
@@ -29136,7 +29142,7 @@
     </row>
     <row r="218" spans="1:92" s="8" customFormat="1">
       <c r="A218" s="38" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B218" s="7"/>
       <c r="E218" s="28"/>
@@ -29197,13 +29203,13 @@
         <v>17</v>
       </c>
       <c r="D219" s="13" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E219" s="6" t="s">
         <v>79</v>
       </c>
       <c r="F219" s="13" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="G219" s="13" t="s">
         <v>115</v>
@@ -29467,19 +29473,19 @@
         <v>3</v>
       </c>
       <c r="B220" s="22" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C220" s="21" t="s">
         <v>7</v>
       </c>
       <c r="D220" s="20" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E220" s="19" t="s">
         <v>3</v>
       </c>
       <c r="F220" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="G220" s="5" t="s">
         <v>177</v>
@@ -29513,7 +29519,7 @@
         <v>3</v>
       </c>
       <c r="R220" s="12" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="S220" s="5" t="s">
         <v>3</v>
@@ -29522,10 +29528,10 @@
         <v>185</v>
       </c>
       <c r="U220" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="V220" s="5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="W220" s="12" t="s">
         <v>228</v>
@@ -29641,7 +29647,7 @@
     </row>
     <row r="222" spans="1:92" s="8" customFormat="1">
       <c r="A222" s="38" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B222" s="7"/>
       <c r="E222" s="28"/>
@@ -29756,7 +29762,7 @@
         <v>27</v>
       </c>
       <c r="V223" s="16" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="W223" s="16" t="s">
         <v>28</v>
@@ -29972,19 +29978,19 @@
         <v>3</v>
       </c>
       <c r="B224" s="22" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C224" s="21" t="s">
         <v>7</v>
       </c>
       <c r="D224" s="5" t="s">
-        <v>237</v>
+        <v>343</v>
       </c>
       <c r="E224" s="19" t="s">
         <v>175</v>
       </c>
       <c r="F224" s="5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="G224" s="5" t="s">
         <v>177</v>
@@ -30018,7 +30024,7 @@
         <v>3</v>
       </c>
       <c r="R224" s="12" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="S224" s="5" t="s">
         <v>3</v>
@@ -30027,10 +30033,10 @@
         <v>185</v>
       </c>
       <c r="U224" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="V224" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="W224" s="12" t="s">
         <v>228</v>
@@ -30146,7 +30152,7 @@
     </row>
     <row r="226" spans="1:92" s="8" customFormat="1">
       <c r="A226" s="38" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B226" s="7"/>
       <c r="E226" s="28"/>
@@ -30261,7 +30267,7 @@
         <v>27</v>
       </c>
       <c r="V227" s="16" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="W227" s="16" t="s">
         <v>28</v>
@@ -30477,19 +30483,19 @@
         <v>3</v>
       </c>
       <c r="B228" s="22" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C228" s="21" t="s">
         <v>7</v>
       </c>
       <c r="D228" s="5" t="s">
-        <v>237</v>
+        <v>343</v>
       </c>
       <c r="E228" s="19" t="s">
         <v>175</v>
       </c>
       <c r="F228" s="5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="G228" s="5" t="s">
         <v>177</v>
@@ -30523,7 +30529,7 @@
         <v>3</v>
       </c>
       <c r="R228" s="12" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="S228" s="5" t="s">
         <v>3</v>
@@ -30532,10 +30538,10 @@
         <v>185</v>
       </c>
       <c r="U228" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="V228" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="W228" s="12" t="s">
         <v>228</v>
@@ -30646,10 +30652,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="229" spans="1:92" ht="409.6">
+    <row r="229" spans="1:92">
       <c r="E229" s="31"/>
     </row>
-    <row r="230" spans="1:92" s="8" customFormat="1" ht="409.6">
+    <row r="230" spans="1:92" s="8" customFormat="1">
       <c r="A230" s="38" t="s">
         <v>205</v>
       </c>
@@ -30988,13 +30994,13 @@
         <v>7</v>
       </c>
       <c r="D232" s="5" t="s">
-        <v>237</v>
+        <v>343</v>
       </c>
       <c r="E232" s="19" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F232" s="5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="G232" s="5" t="s">
         <v>177</v>
@@ -31035,10 +31041,10 @@
         <v>203</v>
       </c>
       <c r="U232" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="V232" s="5" t="s">
         <v>250</v>
-      </c>
-      <c r="V232" s="5" t="s">
-        <v>251</v>
       </c>
       <c r="W232" s="12" t="s">
         <v>228</v>
@@ -31149,12 +31155,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="233" spans="1:92" ht="409.6">
+    <row r="233" spans="1:92">
       <c r="E233" s="31"/>
     </row>
-    <row r="234" spans="1:92" s="8" customFormat="1" ht="409.6">
+    <row r="234" spans="1:92" s="8" customFormat="1">
       <c r="A234" s="38" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B234" s="7"/>
       <c r="E234" s="28"/>
@@ -31485,19 +31491,19 @@
         <v>3</v>
       </c>
       <c r="B236" s="22" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C236" s="39" t="s">
         <v>156</v>
       </c>
       <c r="D236" s="5" t="s">
-        <v>237</v>
+        <v>343</v>
       </c>
       <c r="E236" s="19" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F236" s="5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G236" s="5" t="s">
         <v>177</v>
@@ -31538,10 +31544,10 @@
         <v>203</v>
       </c>
       <c r="U236" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="V236" s="5" t="s">
         <v>250</v>
-      </c>
-      <c r="V236" s="5" t="s">
-        <v>251</v>
       </c>
       <c r="W236" s="12" t="s">
         <v>228</v>
@@ -31652,10 +31658,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="237" spans="1:92" ht="409.6">
+    <row r="237" spans="1:92">
       <c r="E237" s="31"/>
     </row>
-    <row r="238" spans="1:92" s="8" customFormat="1" ht="409.6">
+    <row r="238" spans="1:92" s="8" customFormat="1">
       <c r="A238" s="38" t="s">
         <v>201</v>
       </c>
@@ -31983,7 +31989,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="240" spans="1:92" s="5" customFormat="1" ht="38.25">
+    <row r="240" spans="1:92" s="5" customFormat="1" ht="63.75">
       <c r="A240" s="27" t="s">
         <v>3</v>
       </c>
@@ -31991,16 +31997,16 @@
         <v>202</v>
       </c>
       <c r="C240" s="21" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D240" s="5" t="s">
-        <v>237</v>
+        <v>343</v>
       </c>
       <c r="E240" s="19" t="s">
+        <v>331</v>
+      </c>
+      <c r="F240" s="5" t="s">
         <v>332</v>
-      </c>
-      <c r="F240" s="5" t="s">
-        <v>333</v>
       </c>
       <c r="G240" s="5" t="s">
         <v>177</v>
@@ -32022,10 +32028,10 @@
         <v>180</v>
       </c>
       <c r="N240" s="12" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="O240" s="12" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="P240" s="12" t="s">
         <v>122</v>
@@ -32041,10 +32047,10 @@
         <v>203</v>
       </c>
       <c r="U240" s="5" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="V240" s="5" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="W240" s="12" t="s">
         <v>228</v>
@@ -32052,7 +32058,7 @@
       <c r="X240" s="12"/>
       <c r="Y240" s="12"/>
       <c r="Z240" s="12" t="s">
-        <v>3</v>
+        <v>345</v>
       </c>
       <c r="AA240" s="12" t="s">
         <v>29</v>
@@ -32155,10 +32161,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="241" spans="1:92" ht="409.6">
+    <row r="241" spans="1:92">
       <c r="E241" s="31"/>
     </row>
-    <row r="242" spans="1:92" s="8" customFormat="1" ht="409.6">
+    <row r="242" spans="1:92" s="8" customFormat="1">
       <c r="A242" s="38" t="s">
         <v>220</v>
       </c>
@@ -32497,13 +32503,13 @@
         <v>156</v>
       </c>
       <c r="D244" s="5" t="s">
-        <v>237</v>
+        <v>343</v>
       </c>
       <c r="E244" s="19" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F244" s="5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G244" s="5" t="s">
         <v>177</v>
@@ -32544,10 +32550,10 @@
         <v>203</v>
       </c>
       <c r="U244" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="V244" s="5" t="s">
         <v>250</v>
-      </c>
-      <c r="V244" s="5" t="s">
-        <v>251</v>
       </c>
       <c r="W244" s="12" t="s">
         <v>228</v>
@@ -32658,13 +32664,13 @@
         <v>15</v>
       </c>
     </row>
-    <row r="245" spans="1:92" ht="409.6">
+    <row r="245" spans="1:92">
       <c r="E245" s="31"/>
     </row>
-    <row r="246" spans="1:92" ht="409.6">
+    <row r="246" spans="1:92">
       <c r="E246" s="31"/>
     </row>
-    <row r="247" spans="1:92" s="26" customFormat="1" ht="409.6">
+    <row r="247" spans="1:92" s="26" customFormat="1">
       <c r="A247" s="23"/>
       <c r="B247" s="24"/>
       <c r="C247" s="23"/>
@@ -32732,7 +32738,7 @@
       <c r="BO247" s="25"/>
       <c r="BP247" s="25"/>
     </row>
-    <row r="248" spans="1:92" s="26" customFormat="1" ht="409.6">
+    <row r="248" spans="1:92" s="26" customFormat="1">
       <c r="A248" s="23"/>
       <c r="B248" s="24"/>
       <c r="C248" s="23"/>
@@ -32800,7 +32806,7 @@
       <c r="BO248" s="25"/>
       <c r="BP248" s="25"/>
     </row>
-    <row r="249" spans="1:92" s="26" customFormat="1" ht="409.6">
+    <row r="249" spans="1:92" s="26" customFormat="1">
       <c r="A249" s="23"/>
       <c r="B249" s="24"/>
       <c r="C249" s="23"/>
@@ -32868,7 +32874,7 @@
       <c r="BO249" s="25"/>
       <c r="BP249" s="25"/>
     </row>
-    <row r="250" spans="1:92" s="26" customFormat="1" ht="409.6">
+    <row r="250" spans="1:92" s="26" customFormat="1">
       <c r="A250" s="23"/>
       <c r="B250" s="24"/>
       <c r="C250" s="23"/>
@@ -32942,8 +32948,9 @@
     <hyperlink ref="D192" r:id="rId2" display="AJOETEST@GMAIL.COM :: Professional Engineer :: JA&amp; LLC"/>
     <hyperlink ref="AA192" r:id="rId3"/>
     <hyperlink ref="AB192" r:id="rId4"/>
+    <hyperlink ref="D50" r:id="rId5" display="AJOETEST2@GMAIL.COM :: Professional Engineer :: AJ2V"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>